<commit_message>
Feb and parkrun location data
</commit_message>
<xml_diff>
--- a/site/res/json/_Overall-raceData.xlsx
+++ b/site/res/json/_Overall-raceData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\frimleyFlyers\site\res\json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DF621E-736A-4986-B72D-57B9C44FA547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D376E5-D37B-48BB-88AF-5D87101FF895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6D51F29C-25B3-44AC-A010-76881403EF2A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6D51F29C-25B3-44AC-A010-76881403EF2A}"/>
   </bookViews>
   <sheets>
     <sheet name="overall-raceData2024.json" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="102">
   <si>
     <t>Overall</t>
   </si>
@@ -61,129 +61,60 @@
     <t>Steve Page</t>
   </si>
   <si>
-    <t xml:space="preserve">24:47	</t>
-  </si>
-  <si>
     <t>Lewis Whatley</t>
   </si>
   <si>
-    <t xml:space="preserve">19:12	</t>
-  </si>
-  <si>
     <t>Lucy Bass</t>
   </si>
   <si>
-    <t xml:space="preserve">32:04	</t>
-  </si>
-  <si>
-    <t>Zoe Stone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30:10	</t>
-  </si>
-  <si>
     <t>Susan Harvey</t>
   </si>
   <si>
-    <t xml:space="preserve">31:08	</t>
-  </si>
-  <si>
     <t>Karen Peddle</t>
   </si>
   <si>
-    <t xml:space="preserve">40:11	</t>
-  </si>
-  <si>
     <t>Kev Knight</t>
   </si>
   <si>
-    <t xml:space="preserve">23:57	</t>
-  </si>
-  <si>
     <t>Alan Bush</t>
   </si>
   <si>
-    <t xml:space="preserve">20:02	</t>
-  </si>
-  <si>
     <t>Jodie Raynsford</t>
   </si>
   <si>
-    <t xml:space="preserve">27:53	</t>
-  </si>
-  <si>
     <t>Jo Longmuir</t>
   </si>
   <si>
-    <t xml:space="preserve">23:32	</t>
-  </si>
-  <si>
     <t>Matthew Knight</t>
   </si>
   <si>
-    <t xml:space="preserve">22:42	</t>
-  </si>
-  <si>
     <t>Paul Williams</t>
   </si>
   <si>
-    <t xml:space="preserve">20:52	</t>
-  </si>
-  <si>
     <t>Adrian Keane-Munday</t>
   </si>
   <si>
-    <t xml:space="preserve">26:42	</t>
-  </si>
-  <si>
-    <t>Adam Pett</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28:19	</t>
-  </si>
-  <si>
     <t>Sarah Campbell-Foster</t>
   </si>
   <si>
-    <t xml:space="preserve">29:14	</t>
-  </si>
-  <si>
     <t>Martin Gay</t>
   </si>
   <si>
-    <t xml:space="preserve">24:28	</t>
-  </si>
-  <si>
     <t>Alasdair Nuttall</t>
   </si>
   <si>
-    <t xml:space="preserve">24:26	</t>
-  </si>
-  <si>
     <t>Duncan Ball</t>
   </si>
   <si>
-    <t xml:space="preserve">27:18	</t>
-  </si>
-  <si>
     <t>Simon Harvey</t>
   </si>
   <si>
-    <t xml:space="preserve">21:29	</t>
-  </si>
-  <si>
     <t>Harvey Ockrim</t>
   </si>
   <si>
-    <t xml:space="preserve">26:52	</t>
-  </si>
-  <si>
     <t>Kirstie Stone</t>
   </si>
   <si>
-    <t xml:space="preserve">32:26	</t>
-  </si>
-  <si>
     <t>Susan Rodrigues</t>
   </si>
   <si>
@@ -193,75 +124,33 @@
     <t>Wendy Ockrim</t>
   </si>
   <si>
-    <t xml:space="preserve">32:50	</t>
-  </si>
-  <si>
     <t>Andy Poulter</t>
   </si>
   <si>
-    <t xml:space="preserve">21:15	</t>
-  </si>
-  <si>
     <t>Chris Peddle</t>
   </si>
   <si>
-    <t xml:space="preserve">23:53	</t>
-  </si>
-  <si>
     <t>Christine Scally</t>
   </si>
   <si>
-    <t xml:space="preserve">25:42	</t>
-  </si>
-  <si>
     <t>Darren Stone</t>
   </si>
   <si>
-    <t xml:space="preserve">20:27	</t>
-  </si>
-  <si>
-    <t>Em Howden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29:02	</t>
-  </si>
-  <si>
     <t>Fiona Keane-Munday</t>
   </si>
   <si>
-    <t xml:space="preserve">27:49	</t>
-  </si>
-  <si>
     <t>James Ball</t>
   </si>
   <si>
-    <t xml:space="preserve">22:40	</t>
-  </si>
-  <si>
     <t>Karen Phillips</t>
   </si>
   <si>
-    <t xml:space="preserve">24:31	</t>
-  </si>
-  <si>
     <t>Louise McIntosh</t>
   </si>
   <si>
-    <t xml:space="preserve">28:11	</t>
-  </si>
-  <si>
     <t>Paul Bass</t>
   </si>
   <si>
-    <t xml:space="preserve">24:58	</t>
-  </si>
-  <si>
-    <t>Rich Howden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23:05	</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -308,6 +197,135 @@
   </si>
   <si>
     <t>November</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30:52	</t>
+  </si>
+  <si>
+    <t>Ben Gay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24:38	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:56	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20:04	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29:17	</t>
+  </si>
+  <si>
+    <t>Rebecca Williams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30:50	</t>
+  </si>
+  <si>
+    <t>Leonie Harvey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25:44	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:41	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28:00	</t>
+  </si>
+  <si>
+    <t>Charlotte Knight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33:33	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39:18	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32:53	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:13	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29:38	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27:09	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24:40	</t>
+  </si>
+  <si>
+    <t>Ashton Peddle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33:39	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24:59	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26:46	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:11	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28:12	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27:22	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24:34	</t>
+  </si>
+  <si>
+    <t>Jen Knight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33:58	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26:14	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23:30	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32:37	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:09	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30:27	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24:25	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26:44	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20:53	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:33	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30:03	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:38	</t>
+  </si>
+  <si>
+    <t>Tom Churchill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26:50	</t>
   </si>
 </sst>
 </file>
@@ -813,7 +831,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -822,6 +840,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -919,8 +944,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00E5D0C1-CCA7-40C9-9E58-669E7A37AF9B}" name="Table4" displayName="Table4" ref="A1:K37" totalsRowShown="0">
-  <autoFilter ref="A1:K37" xr:uid="{00E5D0C1-CCA7-40C9-9E58-669E7A37AF9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00E5D0C1-CCA7-40C9-9E58-669E7A37AF9B}" name="Table4" displayName="Table4" ref="A1:K40" totalsRowShown="0">
+  <autoFilter ref="A1:K40" xr:uid="{00E5D0C1-CCA7-40C9-9E58-669E7A37AF9B}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{D31C8478-6486-456A-B915-8C622DD34D1F}" name="Column1" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{73333B76-2155-4A40-8BDD-768B05B71D40}" name="Column2" dataDxfId="0"/>
@@ -1269,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40047064-E81B-4E5B-96D8-6D925F1813E0}">
-  <dimension ref="A1:P37"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,52 +1316,52 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="G1" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="I1" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="J1" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="K1" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="L1" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="M1" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="N1" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="O1" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="P1" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -1362,19 +1387,19 @@
         <v>6</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>94</v>
+        <v>57</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -1429,173 +1454,125 @@
     </row>
     <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B4" s="3">
-        <v>174</v>
+        <v>48</v>
       </c>
       <c r="C4" s="4">
-        <v>126</v>
+        <v>26</v>
       </c>
       <c r="D4" s="4">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="F4" s="4">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="G4" s="4">
-        <v>22</v>
-      </c>
-      <c r="H4" s="4">
-        <v>22</v>
-      </c>
-      <c r="I4" s="4">
         <v>26</v>
       </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="4">
-        <v>26</v>
-      </c>
-      <c r="L4" s="4">
-        <v>26</v>
-      </c>
-      <c r="M4" s="4">
-        <v>26</v>
-      </c>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="4">
-        <v>26</v>
-      </c>
+      <c r="O4" s="4"/>
       <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="B5" s="3">
-        <v>115</v>
+        <v>26</v>
       </c>
       <c r="C5" s="4">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="D5" s="4">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="F5" s="4">
         <v>26</v>
       </c>
-      <c r="G5" s="4">
-        <v>19</v>
-      </c>
+      <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="4">
-        <v>22</v>
-      </c>
-      <c r="J5" s="4">
-        <v>22</v>
-      </c>
-      <c r="K5" s="4">
-        <v>0</v>
-      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="4">
-        <v>0</v>
-      </c>
-      <c r="N5" s="4">
-        <v>26</v>
-      </c>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3">
-        <v>97</v>
+        <v>26</v>
       </c>
       <c r="C6" s="4">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="D6" s="4">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="F6" s="4">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G6" s="4">
-        <v>2</v>
-      </c>
-      <c r="H6" s="4">
-        <v>1</v>
-      </c>
-      <c r="I6" s="4">
-        <v>1</v>
-      </c>
-      <c r="J6" s="4">
-        <v>0</v>
-      </c>
-      <c r="K6" s="4">
         <v>12</v>
       </c>
-      <c r="L6" s="4">
-        <v>19</v>
-      </c>
-      <c r="M6" s="4">
-        <v>22</v>
-      </c>
-      <c r="N6" s="4">
-        <v>22</v>
-      </c>
-      <c r="O6" s="4">
-        <v>0</v>
-      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
       <c r="P6" s="4"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4">
+        <v>4</v>
+      </c>
+      <c r="D7" s="4">
         <v>14</v>
       </c>
-      <c r="B7" s="3">
-        <v>90</v>
-      </c>
-      <c r="C7" s="4">
-        <v>65</v>
-      </c>
-      <c r="D7" s="4">
-        <v>25</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="F7" s="4">
-        <v>17</v>
-      </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4">
-        <v>17</v>
-      </c>
-      <c r="I7" s="4">
-        <v>8</v>
-      </c>
-      <c r="J7" s="4">
-        <v>26</v>
-      </c>
-      <c r="K7" s="4">
-        <v>22</v>
-      </c>
-      <c r="L7" s="4">
-        <v>8</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="G7" s="4">
+        <v>14</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
@@ -1603,76 +1580,60 @@
     </row>
     <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B8" s="3">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="C8" s="4">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D8" s="4">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4">
-        <v>4</v>
-      </c>
-      <c r="I8" s="4">
-        <v>15</v>
-      </c>
-      <c r="J8" s="4">
-        <v>8</v>
-      </c>
+      <c r="G8" s="4">
+        <v>17</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="4">
-        <v>22</v>
-      </c>
-      <c r="M8" s="4">
-        <v>12</v>
-      </c>
-      <c r="N8" s="4">
-        <v>8</v>
-      </c>
-      <c r="O8" s="4">
-        <v>17</v>
-      </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="B9" s="3">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="C9" s="4">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="D9" s="4">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="F9" s="4">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G9" s="4">
-        <v>26</v>
-      </c>
-      <c r="H9" s="4">
-        <v>26</v>
-      </c>
-      <c r="I9" s="4">
-        <v>19</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
@@ -1683,469 +1644,331 @@
     </row>
     <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="C10" s="4">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="D10" s="4">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F10" s="4">
-        <v>0</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4">
-        <v>6</v>
-      </c>
-      <c r="I10" s="4">
-        <v>0</v>
-      </c>
-      <c r="J10" s="4">
-        <v>14</v>
-      </c>
-      <c r="K10" s="4">
-        <v>14</v>
-      </c>
-      <c r="L10" s="4">
-        <v>0</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G10" s="4">
+        <v>4</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
       <c r="M10" s="4"/>
-      <c r="N10" s="4">
-        <v>10</v>
-      </c>
-      <c r="O10" s="4">
-        <v>12</v>
-      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
       <c r="P10" s="4"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="B11" s="3">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C11" s="4">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="D11" s="4">
         <v>0</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="F11" s="4">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="G11" s="4">
-        <v>6</v>
-      </c>
-      <c r="H11" s="4">
-        <v>0</v>
-      </c>
-      <c r="I11" s="4">
-        <v>2</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
       <c r="J11" s="4"/>
-      <c r="K11" s="4">
-        <v>0</v>
-      </c>
+      <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
-      <c r="N11" s="4">
-        <v>12</v>
-      </c>
-      <c r="O11" s="4">
-        <v>14</v>
-      </c>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
       <c r="P11" s="4"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C12" s="4">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D12" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="F12" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="4">
-        <v>8</v>
-      </c>
-      <c r="I12" s="4">
-        <v>4</v>
-      </c>
-      <c r="J12" s="4">
-        <v>10</v>
-      </c>
-      <c r="K12" s="4">
-        <v>2</v>
-      </c>
-      <c r="L12" s="4">
-        <v>12</v>
-      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="4">
-        <v>4</v>
-      </c>
-      <c r="O12" s="4">
-        <v>10</v>
-      </c>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
       <c r="P12" s="4"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="3">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="C13" s="4">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D13" s="4">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="4">
-        <v>0</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="F13" s="4"/>
       <c r="G13" s="4">
-        <v>12</v>
-      </c>
-      <c r="H13" s="4">
-        <v>19</v>
-      </c>
-      <c r="I13" s="4">
-        <v>6</v>
-      </c>
-      <c r="J13" s="4">
-        <v>12</v>
-      </c>
-      <c r="K13" s="4">
-        <v>0</v>
-      </c>
-      <c r="L13" s="4">
-        <v>0</v>
-      </c>
-      <c r="M13" s="4">
-        <v>0</v>
-      </c>
-      <c r="N13" s="4">
-        <v>0</v>
-      </c>
-      <c r="O13" s="4">
-        <v>0</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
       <c r="P13" s="4"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="B14" s="3">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="C14" s="4">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D14" s="4">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="F14" s="4">
-        <v>2</v>
-      </c>
-      <c r="G14" s="4">
-        <v>10</v>
-      </c>
-      <c r="H14" s="4">
-        <v>15</v>
-      </c>
-      <c r="I14" s="4">
-        <v>17</v>
-      </c>
-      <c r="J14" s="4">
-        <v>0</v>
-      </c>
-      <c r="K14" s="4">
-        <v>0</v>
-      </c>
-      <c r="L14" s="4">
-        <v>1</v>
-      </c>
-      <c r="M14" s="4">
-        <v>8</v>
-      </c>
-      <c r="N14" s="4">
-        <v>0</v>
-      </c>
-      <c r="O14" s="4">
-        <v>4</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
       <c r="P14" s="4"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B15" s="3">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C15" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D15" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="F15" s="4">
         <v>0</v>
       </c>
       <c r="G15" s="4">
-        <v>0</v>
-      </c>
-      <c r="H15" s="4">
-        <v>0</v>
-      </c>
-      <c r="I15" s="4">
-        <v>0</v>
-      </c>
-      <c r="J15" s="4">
         <v>6</v>
       </c>
-      <c r="K15" s="4">
-        <v>6</v>
-      </c>
-      <c r="L15" s="4">
-        <v>0</v>
-      </c>
-      <c r="M15" s="4">
-        <v>14</v>
-      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
       <c r="N15" s="4"/>
-      <c r="O15" s="4">
-        <v>0</v>
-      </c>
+      <c r="O15" s="4"/>
       <c r="P15" s="4"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C16" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D16" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="F16" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16" s="4">
-        <v>0</v>
-      </c>
-      <c r="H16" s="4">
-        <v>0</v>
-      </c>
-      <c r="I16" s="4">
-        <v>0</v>
-      </c>
-      <c r="J16" s="4">
-        <v>0</v>
-      </c>
-      <c r="K16" s="4">
-        <v>1</v>
-      </c>
-      <c r="L16" s="4">
-        <v>0</v>
-      </c>
-      <c r="M16" s="4">
-        <v>6</v>
-      </c>
-      <c r="N16" s="4">
-        <v>14</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B17" s="3">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C17" s="4">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D17" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="F17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="4">
         <v>0</v>
       </c>
-      <c r="H17" s="4">
-        <v>2</v>
-      </c>
-      <c r="I17" s="4">
-        <v>0</v>
-      </c>
-      <c r="J17" s="4">
-        <v>4</v>
-      </c>
-      <c r="K17" s="4">
-        <v>0</v>
-      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="4">
-        <v>10</v>
-      </c>
-      <c r="N17" s="4">
-        <v>0</v>
-      </c>
-      <c r="O17" s="4">
-        <v>2</v>
-      </c>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
       <c r="P17" s="4"/>
     </row>
     <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="B18" s="3">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C18" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="4">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="F18" s="4">
         <v>0</v>
       </c>
       <c r="G18" s="4">
-        <v>0</v>
-      </c>
-      <c r="H18" s="4">
-        <v>0</v>
-      </c>
-      <c r="I18" s="4">
-        <v>0</v>
-      </c>
-      <c r="J18" s="4">
-        <v>0</v>
-      </c>
-      <c r="K18" s="4">
-        <v>4</v>
-      </c>
-      <c r="L18" s="4">
-        <v>10</v>
-      </c>
-      <c r="M18" s="4">
-        <v>0</v>
-      </c>
-      <c r="N18" s="4">
-        <v>0</v>
-      </c>
-      <c r="O18" s="4">
-        <v>8</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
       <c r="P18" s="4"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B19" s="3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C19" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="4">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4">
-        <v>0</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="4">
-        <v>0</v>
-      </c>
-      <c r="K19" s="4">
-        <v>10</v>
-      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="4">
-        <v>4</v>
-      </c>
-      <c r="N19" s="4">
-        <v>1</v>
-      </c>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B20" s="3">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C20" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D20" s="4">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F20" s="4">
         <v>0</v>
@@ -2154,86 +1977,68 @@
         <v>0</v>
       </c>
       <c r="H20" s="4"/>
-      <c r="I20" s="4">
-        <v>0</v>
-      </c>
-      <c r="J20" s="4">
-        <v>0</v>
-      </c>
-      <c r="K20" s="4">
-        <v>8</v>
-      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
-      <c r="N20" s="4">
-        <v>6</v>
-      </c>
+      <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="B21" s="3">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C21" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D21" s="4">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="F21" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="4">
         <v>0</v>
       </c>
-      <c r="H21" s="4">
-        <v>0</v>
-      </c>
+      <c r="H21" s="4"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="4">
-        <v>1</v>
-      </c>
-      <c r="K21" s="4">
-        <v>0</v>
-      </c>
-      <c r="L21" s="4">
-        <v>6</v>
-      </c>
-      <c r="M21" s="4">
-        <v>0</v>
-      </c>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
       <c r="N21" s="4"/>
-      <c r="O21" s="4">
-        <v>1</v>
-      </c>
+      <c r="O21" s="4"/>
       <c r="P21" s="4"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B22" s="3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C22" s="4">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D22" s="4">
         <v>0</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
       <c r="G22" s="4">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -2247,281 +2052,191 @@
     </row>
     <row r="23" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="B23" s="3">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C23" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="F23" s="4">
         <v>0</v>
       </c>
-      <c r="G23" s="4">
-        <v>0</v>
-      </c>
-      <c r="H23" s="4">
-        <v>0</v>
-      </c>
-      <c r="I23" s="4">
-        <v>0</v>
-      </c>
-      <c r="J23" s="4">
-        <v>0</v>
-      </c>
-      <c r="K23" s="4">
-        <v>0</v>
-      </c>
-      <c r="L23" s="4">
-        <v>0</v>
-      </c>
-      <c r="M23" s="4">
-        <v>1</v>
-      </c>
-      <c r="N23" s="4">
-        <v>0</v>
-      </c>
-      <c r="O23" s="4">
-        <v>6</v>
-      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
       <c r="P23" s="4"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B24" s="3">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C24" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D24" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="F24" s="4">
         <v>0</v>
       </c>
       <c r="G24" s="4">
-        <v>1</v>
-      </c>
-      <c r="H24" s="4">
-        <v>0</v>
-      </c>
-      <c r="I24" s="4">
-        <v>0</v>
-      </c>
-      <c r="J24" s="4">
-        <v>0</v>
-      </c>
-      <c r="K24" s="4">
-        <v>0</v>
-      </c>
-      <c r="L24" s="4">
-        <v>4</v>
-      </c>
-      <c r="M24" s="4">
-        <v>2</v>
-      </c>
-      <c r="N24" s="4">
-        <v>0</v>
-      </c>
-      <c r="O24" s="4">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B25" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C25" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D25" s="4">
         <v>0</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="F25" s="4">
-        <v>4</v>
-      </c>
-      <c r="G25" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
       <c r="H25" s="4"/>
-      <c r="I25" s="4">
-        <v>0</v>
-      </c>
+      <c r="I25" s="4"/>
       <c r="J25" s="4"/>
-      <c r="K25" s="4">
-        <v>0</v>
-      </c>
+      <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
-      <c r="N25" s="4">
-        <v>0</v>
-      </c>
-      <c r="O25" s="4">
-        <v>0</v>
-      </c>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
       <c r="P25" s="4"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="B26" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C26" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D26" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F26" s="4">
-        <v>0</v>
-      </c>
-      <c r="G26" s="4">
-        <v>0</v>
-      </c>
-      <c r="H26" s="4">
-        <v>0</v>
-      </c>
-      <c r="I26" s="4">
-        <v>0</v>
-      </c>
-      <c r="J26" s="4">
-        <v>0</v>
-      </c>
-      <c r="K26" s="4">
-        <v>0</v>
-      </c>
-      <c r="L26" s="4">
-        <v>2</v>
-      </c>
-      <c r="M26" s="4">
-        <v>0</v>
-      </c>
-      <c r="N26" s="4">
-        <v>2</v>
-      </c>
-      <c r="O26" s="4">
-        <v>0</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B27" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C27" s="4">
         <v>0</v>
       </c>
       <c r="D27" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="F27" s="4">
         <v>0</v>
       </c>
       <c r="G27" s="4">
-        <v>4</v>
-      </c>
-      <c r="H27" s="4">
-        <v>0</v>
-      </c>
-      <c r="I27" s="4">
-        <v>0</v>
-      </c>
-      <c r="J27" s="4">
-        <v>0</v>
-      </c>
-      <c r="K27" s="4">
-        <v>0</v>
-      </c>
-      <c r="L27" s="4">
-        <v>0</v>
-      </c>
-      <c r="M27" s="4">
-        <v>0</v>
-      </c>
-      <c r="N27" s="4">
-        <v>0</v>
-      </c>
-      <c r="O27" s="4">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
       <c r="P27" s="4"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="B28" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C28" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D28" s="4">
         <v>0</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="F28" s="4">
         <v>0</v>
       </c>
       <c r="G28" s="4"/>
-      <c r="H28" s="4">
-        <v>0</v>
-      </c>
-      <c r="I28" s="4">
-        <v>0</v>
-      </c>
-      <c r="J28" s="4">
-        <v>2</v>
-      </c>
-      <c r="K28" s="4">
-        <v>0</v>
-      </c>
-      <c r="L28" s="4">
-        <v>0</v>
-      </c>
-      <c r="M28" s="4">
-        <v>0</v>
-      </c>
-      <c r="N28" s="4">
-        <v>0</v>
-      </c>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B29" s="3">
         <v>0</v>
@@ -2533,37 +2248,27 @@
         <v>0</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="F29" s="4">
         <v>0</v>
       </c>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4">
-        <v>0</v>
-      </c>
-      <c r="I29" s="4">
-        <v>0</v>
-      </c>
+      <c r="G29" s="4">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
       <c r="J29" s="4"/>
-      <c r="K29" s="4">
-        <v>0</v>
-      </c>
+      <c r="K29" s="4"/>
       <c r="L29" s="4"/>
-      <c r="M29" s="4">
-        <v>0</v>
-      </c>
-      <c r="N29" s="4">
-        <v>0</v>
-      </c>
-      <c r="O29" s="4">
-        <v>0</v>
-      </c>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="B30" s="3">
         <v>0</v>
@@ -2575,37 +2280,25 @@
         <v>0</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="F30" s="4">
         <v>0</v>
       </c>
       <c r="G30" s="4"/>
-      <c r="H30" s="4">
-        <v>0</v>
-      </c>
+      <c r="H30" s="4"/>
       <c r="I30" s="4"/>
-      <c r="J30" s="4">
-        <v>0</v>
-      </c>
-      <c r="K30" s="4">
-        <v>0</v>
-      </c>
-      <c r="L30" s="4">
-        <v>0</v>
-      </c>
-      <c r="M30" s="4">
-        <v>0</v>
-      </c>
-      <c r="N30" s="4">
-        <v>0</v>
-      </c>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3">
         <v>0</v>
@@ -2617,10 +2310,14 @@
         <v>0</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+        <v>91</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0</v>
+      </c>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
@@ -2633,7 +2330,7 @@
     </row>
     <row r="32" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="B32" s="3">
         <v>0</v>
@@ -2645,7 +2342,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="F32" s="4">
         <v>0</v>
@@ -2655,23 +2352,17 @@
       </c>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
-      <c r="J32" s="4">
-        <v>0</v>
-      </c>
-      <c r="K32" s="4">
-        <v>0</v>
-      </c>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
       <c r="L32" s="4"/>
-      <c r="M32" s="4">
-        <v>0</v>
-      </c>
+      <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
     </row>
     <row r="33" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="B33" s="3">
         <v>0</v>
@@ -2683,39 +2374,25 @@
         <v>0</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="F33" s="4">
         <v>0</v>
       </c>
-      <c r="G33" s="4">
-        <v>0</v>
-      </c>
-      <c r="H33" s="4">
-        <v>0</v>
-      </c>
-      <c r="I33" s="4">
-        <v>0</v>
-      </c>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
       <c r="J33" s="4"/>
-      <c r="K33" s="4">
-        <v>0</v>
-      </c>
-      <c r="L33" s="4">
-        <v>0</v>
-      </c>
-      <c r="M33" s="4">
-        <v>0</v>
-      </c>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
       <c r="N33" s="4"/>
-      <c r="O33" s="4">
-        <v>0</v>
-      </c>
+      <c r="O33" s="4"/>
       <c r="P33" s="4"/>
     </row>
     <row r="34" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="B34" s="3">
         <v>0</v>
@@ -2727,11 +2404,9 @@
         <v>0</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F34" s="4">
-        <v>0</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="F34" s="4"/>
       <c r="G34" s="4">
         <v>0</v>
       </c>
@@ -2747,7 +2422,7 @@
     </row>
     <row r="35" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="B35" s="3">
         <v>0</v>
@@ -2759,41 +2434,23 @@
         <v>0</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F35" s="4">
-        <v>0</v>
-      </c>
-      <c r="G35" s="4">
-        <v>0</v>
-      </c>
-      <c r="H35" s="4">
-        <v>0</v>
-      </c>
-      <c r="I35" s="4">
-        <v>0</v>
-      </c>
-      <c r="J35" s="4">
-        <v>0</v>
-      </c>
-      <c r="K35" s="4">
-        <v>0</v>
-      </c>
-      <c r="L35" s="4">
-        <v>0</v>
-      </c>
-      <c r="M35" s="4">
-        <v>0</v>
-      </c>
-      <c r="N35" s="4">
-        <v>0</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="B36" s="3">
         <v>0</v>
@@ -2805,7 +2462,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F36" s="4">
         <v>0</v>
@@ -2814,28 +2471,18 @@
         <v>0</v>
       </c>
       <c r="H36" s="4"/>
-      <c r="I36" s="4">
-        <v>0</v>
-      </c>
-      <c r="J36" s="4">
-        <v>0</v>
-      </c>
-      <c r="K36" s="4">
-        <v>0</v>
-      </c>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
       <c r="L36" s="4"/>
-      <c r="M36" s="4">
-        <v>0</v>
-      </c>
-      <c r="N36" s="4">
-        <v>0</v>
-      </c>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
     </row>
     <row r="37" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="B37" s="3">
         <v>0</v>
@@ -2847,10 +2494,14 @@
         <v>0</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+        <v>97</v>
+      </c>
+      <c r="F37" s="4">
+        <v>0</v>
+      </c>
+      <c r="G37" s="4">
+        <v>0</v>
+      </c>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
@@ -2861,12 +2512,103 @@
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
     </row>
+    <row r="38" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="7">
+        <v>0</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0</v>
+      </c>
+      <c r="D38" s="6">
+        <v>0</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F38" s="6">
+        <v>0</v>
+      </c>
+      <c r="G38" s="6">
+        <v>0</v>
+      </c>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="6"/>
+    </row>
+    <row r="39" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="7">
+        <v>0</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0</v>
+      </c>
+      <c r="D39" s="6">
+        <v>0</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6">
+        <v>0</v>
+      </c>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+    </row>
+    <row r="40" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B40" s="7">
+        <v>0</v>
+      </c>
+      <c r="C40" s="6">
+        <v>0</v>
+      </c>
+      <c r="D40" s="6">
+        <v>0</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="6"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>